<commit_message>
aggiunti file challenge 3
</commit_message>
<xml_diff>
--- a/project1/parking duty cycle.xlsx
+++ b/project1/parking duty cycle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D03AC01-3819-4DF2-BF5B-D6F47F52055C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9F0F99-DE85-40AF-8C83-5016BFCF91BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7836" xr2:uid="{976D03B0-1215-4A28-A036-C8101FB24F99}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>boot</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>time of life seconds</t>
+  </si>
+  <si>
+    <t>turning wifi off</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2C0BD1-AF70-4BAD-A95A-07E16DB09CD9}">
-  <dimension ref="C3:J17"/>
+  <dimension ref="C3:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +492,7 @@
         <v>466.74400000000003</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5:F9" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F10" si="0">D5*E5</f>
         <v>1.16686</v>
       </c>
       <c r="G5" s="1"/>
@@ -544,77 +547,93 @@
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D9">
-        <v>120</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
+        <v>5.1450000000000003E-3</v>
+      </c>
+      <c r="E9" s="7">
+        <v>775.5</v>
+      </c>
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.9899475000000004</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5">
+        <v>59.66</v>
       </c>
       <c r="F10" s="6">
-        <f>SUM(F4:F9)</f>
-        <v>59.266938219219711</v>
+        <f t="shared" si="0"/>
+        <v>417.62</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="I10">
-        <f>F9/F10</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6">
+        <f>SUM(F4:F10)</f>
+        <v>480.87688571921973</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="I11">
+        <f>F10/F11</f>
+        <v>0.86845513353254633</v>
+      </c>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D11">
-        <f>SUM(D4:D9)</f>
-        <v>120.187262</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+      <c r="D12">
+        <f>SUM(D4:D10)</f>
+        <v>7.1924070000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>18402000</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D15">
-        <f>D13/F10</f>
-        <v>310493.51548976096</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="2" t="s">
+      <c r="D16">
+        <f>D14/F11</f>
+        <v>38267.591033154349</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="9">
-        <f>D15*D11</f>
-        <v>37317365.495468959</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+      <c r="D17" s="9">
+        <f>D16*D12</f>
+        <v>275236.08961999661</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D17">
-        <f>D16/3600</f>
-        <v>10365.934859852488</v>
+      <c r="D18">
+        <f>D17/3600</f>
+        <v>76.454469338887947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>